<commit_message>
Added CCLI numbers to Hillsong, WOW. Added MaranathaMusic, Artists sheet.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/Passion/Passion.xlsx
+++ b/WorshipCreator.TestData/Source/Books/Passion/Passion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\Passion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5838EE48-96C4-4FD7-8004-7C833A4B46D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8D0C50-B46A-449B-B469-F081C56D8952}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3435" yWindow="3435" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{6DC4884E-2255-4F3E-AC7B-A47A80FF60B1}"/>
+    <workbookView xWindow="31785" yWindow="2985" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{6DC4884E-2255-4F3E-AC7B-A47A80FF60B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Albums" sheetId="1" r:id="rId1"/>
@@ -1504,21 +1504,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -5596,9 +5582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F19F2C-901C-4BEF-AD03-4779E7C45D4C}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6248,8 +6234,8 @@
   <dimension ref="A1:L324"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J324" sqref="J324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14192,7 +14178,7 @@
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16039,10 +16025,10 @@
     <sortCondition ref="D2:D104"/>
   </sortState>
   <conditionalFormatting sqref="J1">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>